<commit_message>
docs: add spread sheet
performance comparison sheet is added
</commit_message>
<xml_diff>
--- a/spreadsheet.xlsx
+++ b/spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\3secondz\SFND_3D_Object_Tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{781EC532-330F-4753-94BB-0F8AC36DC3B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3F9524-3E18-43E7-9121-5B451D9AE7F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23175" windowHeight="11985" xr2:uid="{3F558E8C-EBAB-4461-B83F-301EB26498CD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5835" windowHeight="11295" xr2:uid="{3F558E8C-EBAB-4461-B83F-301EB26498CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>SHITOMASI-BRISK</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -56,10 +56,6 @@
   </si>
   <si>
     <t>ORB-BRISK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -137,6 +133,1951 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ko-KR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR"/>
+              <a:t>TTC</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LIDAR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$S$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>12.51</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.61</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.09</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.68</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.74</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.78</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.98</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.12</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.02</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.9499999999999993</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.9600000000000009</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.59</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.52</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.51</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.61</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.39</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F3FC-453A-AFF4-B51ED33FA265}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SHITOMASI-BRISK</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$S$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>14.56</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.41</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.08</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.08</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.57</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.01</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.31</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.87</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.48</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11.19</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.88</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.96</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10.09</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11.9</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.73</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F3FC-453A-AFF4-B51ED33FA265}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SHITOMASI-BRIEF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$S$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>11.33</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.92</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.55</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.66</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.05</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.119999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.31</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.84</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.220000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11.17</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.83</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11.16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12.01</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10.62</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.47</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F3FC-453A-AFF4-B51ED33FA265}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SHITOMASI-ORB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$6:$S$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>14.56</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.55</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.55</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.24</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.13</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.039999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.72</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.9499999999999993</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.53</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.83</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.69</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12.19</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10.039999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.92</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F3FC-453A-AFF4-B51ED33FA265}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FAST-BRISK</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$7:$S$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.54</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.98</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.65</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.05</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.47</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.23</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.21</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11.58</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10.65</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10.220000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-F3FC-453A-AFF4-B51ED33FA265}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FAST-BRIEF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$8:$S$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>10.17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.37</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.47</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.95</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10.17</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11.11</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.95</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-F3FC-453A-AFF4-B51ED33FA265}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FAST-ORB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$9:$S$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>11.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.03</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.96</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.45</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.02</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10.4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11.58</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-F3FC-453A-AFF4-B51ED33FA265}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ORB-BRISK</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$S$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>13.87</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26.23</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.61</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.85</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.92</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.02</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.19</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.4700000000000006</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.78</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.28</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.08</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>14.49</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-F3FC-453A-AFF4-B51ED33FA265}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ORB-BRIEF</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$S$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>24.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>63.49</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.03</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.93</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.989999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45.56</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>106.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16.07</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14.11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.82</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12.22</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17.350000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11.62</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.92</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-F3FC-453A-AFF4-B51ED33FA265}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ORB-ORB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$12:$S$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1116</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.52</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>123.35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62.54</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.2799999999999994</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23.15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.63</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.86</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15.76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-F3FC-453A-AFF4-B51ED33FA265}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1353951472"/>
+        <c:axId val="1323421552"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1353951472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1323421552"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1323421552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="30"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ko-KR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1353951472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ko-KR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ko-KR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="차트 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2388FE02-7827-4C20-91F3-F758DB1F1EB1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -436,10 +2377,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19370254-F3DA-4954-816A-CFCAB44CC413}">
-  <dimension ref="A3:T13"/>
+  <dimension ref="A3:T12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="R41" sqref="R41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -506,7 +2447,7 @@
         <v>8.39</v>
       </c>
       <c r="T3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
@@ -942,13 +2883,10 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>24.4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
       </c>
       <c r="D11">
         <v>63.49</v>
@@ -1001,7 +2939,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12">
         <v>1116</v>
@@ -1047,16 +2985,12 @@
       </c>
       <c r="T12">
         <v>275.8725</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="T13">
-        <v>3.343438136324429</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>